<commit_message>
added artikel cara menggunakan metode maut dan excel skema
</commit_message>
<xml_diff>
--- a/TA R8 NOW/Lembar Survey.xlsx
+++ b/TA R8 NOW/Lembar Survey.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_ELDI FOLDER_\_Kuliah\Semester 7\TA hehehehehehe\TA R8 NOW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_ELDI FOLDER_\_Kuliah\Semester 7\TA hehehehehehe\TA-Proposal\TA R8 NOW\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lembar Survey" sheetId="1" r:id="rId1"/>
+    <sheet name="Skema" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
   <si>
     <t>NO</t>
   </si>
@@ -267,13 +268,128 @@
   </si>
   <si>
     <t>Alamat             :        .............................................................................................................................................................................</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Kriteria</t>
+  </si>
+  <si>
+    <t>Bobot Kriteria</t>
+  </si>
+  <si>
+    <t>Produk</t>
+  </si>
+  <si>
+    <t>Pelayanan</t>
+  </si>
+  <si>
+    <t>Pengelolaan</t>
+  </si>
+  <si>
+    <t>KRITERIA DAN BOBOT</t>
+  </si>
+  <si>
+    <t>Alternatif</t>
+  </si>
+  <si>
+    <t>Tidak Syariah</t>
+  </si>
+  <si>
+    <t>Kurang Syariah</t>
+  </si>
+  <si>
+    <t>Syariah</t>
+  </si>
+  <si>
+    <t>Sangat Syariah</t>
+  </si>
+  <si>
+    <t>Kode</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>ALTERNATIF</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>*Preferensi Total bobot =1</t>
+  </si>
+  <si>
+    <t>Presepsi Penilaian</t>
+  </si>
+  <si>
+    <t>Bobot</t>
+  </si>
+  <si>
+    <t>0,25-0,9</t>
+  </si>
+  <si>
+    <t>Hotel A</t>
+  </si>
+  <si>
+    <t>Hotel B</t>
+  </si>
+  <si>
+    <t>Hotel C</t>
+  </si>
+  <si>
+    <t>Hotel D</t>
+  </si>
+  <si>
+    <t>DATA PENILAIAN</t>
+  </si>
+  <si>
+    <t>Responden</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,8 +398,38 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,8 +442,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -357,11 +509,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -385,25 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -422,11 +590,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,6 +667,312 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2085975" y="866775"/>
+          <a:ext cx="1276350" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6086475" y="1190625"/>
+          <a:ext cx="0" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6934200" y="847725"/>
+          <a:ext cx="2028825" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6924675" y="838200"/>
+          <a:ext cx="2028825" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6924675" y="828675"/>
+          <a:ext cx="2076450" cy="2228850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6924675" y="838200"/>
+          <a:ext cx="2066925" cy="3562350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -705,47 +1238,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="4.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29" style="16" customWidth="1"/>
-    <col min="5" max="5" width="4.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.21875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29" style="10" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:13" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:13" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="4" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="4" spans="1:13" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -768,20 +1304,27 @@
         <v>4</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" s="37" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="J4" s="12"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2">
@@ -793,13 +1336,17 @@
       <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="13"/>
+      <c r="H5" s="8">
+        <f ca="1">RANDBETWEEN(0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="36"/>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -809,15 +1356,19 @@
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="9">
+      <c r="H6" s="8">
+        <f t="shared" ref="H6:H53" ca="1" si="0">RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="17">
         <v>2</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="21" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2">
@@ -829,13 +1380,17 @@
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="H7" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="2">
         <v>4</v>
       </c>
@@ -845,13 +1400,18 @@
       <c r="G8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
+      <c r="H8" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="2">
         <v>5</v>
       </c>
@@ -861,13 +1421,17 @@
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="13"/>
+      <c r="H9" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="2">
         <v>6</v>
       </c>
@@ -877,15 +1441,19 @@
       <c r="G10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="9">
+      <c r="H10" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="17">
         <v>3</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="21" t="s">
         <v>58</v>
       </c>
       <c r="E11" s="2">
@@ -897,13 +1465,17 @@
       <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
+      <c r="H11" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="2">
         <v>8</v>
       </c>
@@ -913,13 +1485,17 @@
       <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="13"/>
+      <c r="H12" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="2">
         <v>9</v>
       </c>
@@ -929,15 +1505,19 @@
       <c r="G13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="9">
+      <c r="H13" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="17">
         <v>4</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="21" t="s">
         <v>59</v>
       </c>
       <c r="E14" s="2">
@@ -949,13 +1529,17 @@
       <c r="G14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="13"/>
+      <c r="H14" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="2">
         <v>11</v>
       </c>
@@ -965,15 +1549,19 @@
       <c r="G15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="9">
+      <c r="H15" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="17">
         <v>5</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="21" t="s">
         <v>60</v>
       </c>
       <c r="E16" s="2">
@@ -985,13 +1573,17 @@
       <c r="G16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
+      <c r="H16" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="2">
         <v>13</v>
       </c>
@@ -1001,13 +1593,17 @@
       <c r="G17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
+      <c r="H17" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="2">
         <v>14</v>
       </c>
@@ -1017,13 +1613,17 @@
       <c r="G18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="13"/>
+      <c r="H18" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="2">
         <v>15</v>
       </c>
@@ -1033,15 +1633,19 @@
       <c r="G19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="9">
+      <c r="H19" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="17">
         <v>6</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="21" t="s">
         <v>61</v>
       </c>
       <c r="E20" s="2">
@@ -1053,13 +1657,17 @@
       <c r="G20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
+      <c r="H20" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="2">
         <v>17</v>
       </c>
@@ -1069,13 +1677,17 @@
       <c r="G21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
+      <c r="H21" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="2">
         <v>18</v>
       </c>
@@ -1085,13 +1697,17 @@
       <c r="G22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15"/>
+      <c r="H22" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="2">
         <v>19</v>
       </c>
@@ -1101,13 +1717,17 @@
       <c r="G23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
+      <c r="H23" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="2">
         <v>20</v>
       </c>
@@ -1117,13 +1737,17 @@
       <c r="G24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="15"/>
+      <c r="H24" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="2">
         <v>21</v>
       </c>
@@ -1133,13 +1757,17 @@
       <c r="G25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
+      <c r="H25" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="2">
         <v>22</v>
       </c>
@@ -1149,13 +1777,17 @@
       <c r="G26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
+      <c r="H26" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="2">
         <v>23</v>
       </c>
@@ -1165,13 +1797,17 @@
       <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="13"/>
+      <c r="H27" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="2">
         <v>24</v>
       </c>
@@ -1181,15 +1817,19 @@
       <c r="G28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
+      <c r="H28" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="2">
         <v>7</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E29" s="2">
@@ -1201,15 +1841,19 @@
       <c r="G29" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="9">
+      <c r="H29" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="17">
         <v>8</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="21" t="s">
         <v>63</v>
       </c>
       <c r="E30" s="2">
@@ -1221,13 +1865,17 @@
       <c r="G30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="13"/>
+      <c r="H30" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="2">
         <v>27</v>
       </c>
@@ -1237,19 +1885,26 @@
       <c r="G31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+      <c r="H31" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="35">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="17">
         <v>9</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="21" t="s">
         <v>64</v>
       </c>
       <c r="E32" s="2">
@@ -1261,13 +1916,17 @@
       <c r="G32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15"/>
+      <c r="H32" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="2">
         <v>29</v>
       </c>
@@ -1277,13 +1936,17 @@
       <c r="G33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
+      <c r="H33" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="2">
         <v>30</v>
       </c>
@@ -1293,13 +1956,17 @@
       <c r="G34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
+      <c r="H34" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="2">
         <v>31</v>
       </c>
@@ -1309,13 +1976,17 @@
       <c r="G35" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="13"/>
+      <c r="H35" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="2">
         <v>32</v>
       </c>
@@ -1325,15 +1996,19 @@
       <c r="G36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="9">
+      <c r="H36" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="17">
         <v>10</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="21" t="s">
         <v>65</v>
       </c>
       <c r="E37" s="2">
@@ -1345,13 +2020,17 @@
       <c r="G37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="15"/>
+      <c r="H37" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="2">
         <v>34</v>
       </c>
@@ -1361,13 +2040,17 @@
       <c r="G38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="13"/>
+      <c r="H38" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="22"/>
       <c r="E39" s="2">
         <v>35</v>
       </c>
@@ -1377,15 +2060,19 @@
       <c r="G39" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="9">
+      <c r="H39" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="17">
         <v>11</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="21" t="s">
         <v>66</v>
       </c>
       <c r="E40" s="2">
@@ -1397,13 +2084,17 @@
       <c r="G40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="15"/>
+      <c r="H40" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="23"/>
       <c r="E41" s="2">
         <v>37</v>
       </c>
@@ -1413,13 +2104,17 @@
       <c r="G41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="13"/>
+      <c r="H41" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="2">
         <v>38</v>
       </c>
@@ -1429,15 +2124,19 @@
       <c r="G42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="9">
+      <c r="H42" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="17">
         <v>12</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="21" t="s">
         <v>67</v>
       </c>
       <c r="E43" s="2">
@@ -1449,13 +2148,17 @@
       <c r="G43" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="13"/>
+      <c r="H43" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="2">
         <v>40</v>
       </c>
@@ -1465,15 +2168,19 @@
       <c r="G44" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="9">
+      <c r="H44" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="17">
         <v>13</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E45" s="2">
@@ -1485,13 +2192,17 @@
       <c r="G45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="15"/>
+      <c r="H45" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="23"/>
       <c r="E46" s="2">
         <v>42</v>
       </c>
@@ -1501,13 +2212,17 @@
       <c r="G46" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="15"/>
+      <c r="H46" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="23"/>
       <c r="E47" s="2">
         <v>43</v>
       </c>
@@ -1517,13 +2232,17 @@
       <c r="G47" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="15"/>
+      <c r="H47" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="23"/>
       <c r="E48" s="2">
         <v>44</v>
       </c>
@@ -1533,13 +2252,17 @@
       <c r="G48" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="13"/>
+      <c r="H48" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="8"/>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="2">
         <v>45</v>
       </c>
@@ -1549,15 +2272,19 @@
       <c r="G49" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="9">
+      <c r="H49" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="17">
         <v>14</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="21" t="s">
         <v>69</v>
       </c>
       <c r="E50" s="2">
@@ -1569,13 +2296,17 @@
       <c r="G50" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="13"/>
+      <c r="H50" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I50" s="8"/>
+    </row>
+    <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="22"/>
       <c r="E51" s="2">
         <v>47</v>
       </c>
@@ -1585,19 +2316,26 @@
       <c r="G51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
+      <c r="H51" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="8"/>
+      <c r="J51" s="35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="16" t="s">
         <v>76</v>
       </c>
       <c r="C52" s="2">
         <v>15</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E52" s="2">
@@ -1609,15 +2347,19 @@
       <c r="G52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
+      <c r="H52" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="8"/>
+    </row>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
       <c r="C53" s="2">
         <v>16</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D53" s="9" t="s">
         <v>71</v>
       </c>
       <c r="E53" s="2">
@@ -1629,132 +2371,170 @@
       <c r="G53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="17"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="17"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="17"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="17"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="17"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="17"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="17"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="17"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="17"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="17"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="17"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="17"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="17"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="17"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="17"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="17"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="17"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="17"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="17"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="17"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="17"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="17"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="17"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="17"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="17"/>
+      <c r="H53" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="8"/>
+      <c r="J53" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D20:D28"/>
+    <mergeCell ref="C20:C28"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="C37:C39"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="B52:B53"/>
     <mergeCell ref="B5:B31"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="A5:A31"/>
@@ -1766,26 +2546,412 @@
     <mergeCell ref="C43:C44"/>
     <mergeCell ref="D45:D49"/>
     <mergeCell ref="C45:C49"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D20:D28"/>
-    <mergeCell ref="C20:C28"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="C11:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P28"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="M1" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G2" s="1"/>
+      <c r="N2" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="O2" s="31"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="33"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N9" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="O9" s="31"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H10" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="N10" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="O10" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P10" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H11" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="J11" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H12" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="29"/>
+      <c r="J12" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H13" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="29"/>
+      <c r="J13" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H14" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="29"/>
+      <c r="J14" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N16" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="O16" s="31"/>
+    </row>
+    <row r="17" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M17" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="O17" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P17" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M18" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M20" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="23" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="N23" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="O23" s="32"/>
+    </row>
+    <row r="24" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M24" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="N24" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="O24" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P24" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M25" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M26" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M27" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M28" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>